<commit_message>
feat: complete candidate workflow, resume upload, job linking & HR elite mode base - Candidate create/update stabilized - Cloudinary resume upload & UI filename preview - Exam assign/reassign & email send flows - Exam + department + job joins - Fixed job FK association (jobId) - Added pagination, filters, modals & skeleton UI
</commit_message>
<xml_diff>
--- a/TalentGate + HRMS.xlsx
+++ b/TalentGate + HRMS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>TALENT GATE – MASTER FUNCTIONALITY CHECKLIST</t>
   </si>
@@ -54,21 +54,6 @@
     <t>JOB MANAGEMENT</t>
   </si>
   <si>
-    <t>⬜ Create Job Opening</t>
-  </si>
-  <si>
-    <t>⬜ Edit / Close Job</t>
-  </si>
-  <si>
-    <t>⬜ Define Skills required</t>
-  </si>
-  <si>
-    <t>⬜ Attach Exam to Job</t>
-  </si>
-  <si>
-    <t>⬜ Job listing &amp; status</t>
-  </si>
-  <si>
     <t>CANDIDATE PIPELINE</t>
   </si>
   <si>
@@ -292,13 +277,34 @@
   </si>
   <si>
     <t>⬜ Workflow engine</t>
+  </si>
+  <si>
+    <t>✅ Create Job Opening</t>
+  </si>
+  <si>
+    <t>✅ Edit / Close Job</t>
+  </si>
+  <si>
+    <t>✅ Define Skills required</t>
+  </si>
+  <si>
+    <t>✅ Attach Exam to Job</t>
+  </si>
+  <si>
+    <t>✅ Job listing &amp; status</t>
+  </si>
+  <si>
+    <t>We saved candidates data in website DB</t>
+  </si>
+  <si>
+    <t>Where we have Resume, candidate data etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,13 +312,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -327,13 +359,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,487 +676,532 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:L133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133:XFD133"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="4" width="52.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="4:12">
-      <c r="H2" s="1" t="s">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="4" spans="4:12">
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="4:12">
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="4:12">
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="4:12">
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="4:12">
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="4:12">
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="4:12">
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="4:12">
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="4:12">
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="16" spans="4:12">
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="4:7">
+      <c r="D17" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" s="2" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="4:7">
+      <c r="D18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="4:7">
+      <c r="D19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="4:7">
+      <c r="D20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="4:7">
+      <c r="D21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="4:7">
+      <c r="D22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="25" spans="4:7">
+      <c r="D25" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" s="2" t="s">
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="4:7">
+      <c r="D26" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="4:4">
-      <c r="D20" s="2" t="s">
+      <c r="E26" s="6"/>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="4:7">
+      <c r="D27" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" s="2" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="4:7">
+      <c r="D28" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="4:4">
-      <c r="D22" s="2" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="4:7">
+      <c r="D29" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="4:4">
-      <c r="D25" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="32" spans="4:7">
+      <c r="D32" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4">
-      <c r="D27" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4">
-      <c r="D28" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4">
-      <c r="D29" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4">
-      <c r="D32" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="4:4">
       <c r="D37" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="4:4">
       <c r="D40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="4:4">
       <c r="D41" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="4:4">
       <c r="D42" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="4:4">
       <c r="D43" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="4:4">
       <c r="D44" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="4:4">
       <c r="D47" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="4:4">
-      <c r="D48" s="2" t="s">
-        <v>34</v>
+      <c r="D48" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="4:4">
-      <c r="D49" s="2" t="s">
-        <v>35</v>
+      <c r="D49" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="4:4">
-      <c r="D50" s="2" t="s">
-        <v>36</v>
+      <c r="D50" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="4:4">
-      <c r="D51" s="2" t="s">
-        <v>37</v>
+      <c r="D51" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="4:4">
       <c r="D55" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="4:4">
       <c r="D56" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="4:4">
-      <c r="D57" s="2" t="s">
-        <v>40</v>
+      <c r="D57" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="4:4">
-      <c r="D58" s="2" t="s">
-        <v>41</v>
+      <c r="D58" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="4:4">
-      <c r="D59" s="2" t="s">
-        <v>42</v>
+      <c r="D59" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="4:4">
       <c r="D62" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="4:4">
-      <c r="D63" s="2" t="s">
-        <v>44</v>
+      <c r="D63" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="4:4">
-      <c r="D64" s="2" t="s">
-        <v>45</v>
+      <c r="D64" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="4:4">
-      <c r="D65" s="2" t="s">
-        <v>46</v>
+      <c r="D65" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="4:4">
       <c r="D69" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="4:4">
       <c r="D70" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="4:4">
       <c r="D71" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="4:4">
       <c r="D72" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="4:4">
       <c r="D73" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="4:4">
       <c r="D74" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="4:4">
       <c r="D77" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="4:4">
       <c r="D78" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="4:4">
       <c r="D79" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="4:4">
       <c r="D80" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="4:4">
       <c r="D84" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="85" spans="4:4">
       <c r="D85" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="86" spans="4:4">
-      <c r="D86" s="2" t="s">
-        <v>59</v>
+      <c r="D86" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="4:4">
-      <c r="D87" s="2" t="s">
-        <v>60</v>
+      <c r="D87" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="4:4">
-      <c r="D88" s="2" t="s">
-        <v>61</v>
+      <c r="D88" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="89" spans="4:4">
-      <c r="D89" s="2" t="s">
-        <v>62</v>
+      <c r="D89" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="4:4">
       <c r="D92" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="93" spans="4:4">
       <c r="D93" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="94" spans="4:4">
       <c r="D94" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="95" spans="4:4">
       <c r="D95" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="99" spans="4:4">
       <c r="D99" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="100" spans="4:4">
       <c r="D100" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="101" spans="4:4">
       <c r="D101" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="102" spans="4:4">
       <c r="D102" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="103" spans="4:4">
       <c r="D103" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="106" spans="4:4">
       <c r="D106" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="107" spans="4:4">
-      <c r="D107" s="2" t="s">
-        <v>73</v>
+      <c r="D107" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="108" spans="4:4">
-      <c r="D108" s="2" t="s">
-        <v>74</v>
+      <c r="D108" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="4:4">
-      <c r="D109" s="2" t="s">
-        <v>75</v>
+      <c r="D109" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="113" spans="4:4">
       <c r="D113" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="114" spans="4:4">
       <c r="D114" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="115" spans="4:4">
-      <c r="D115" s="2" t="s">
-        <v>78</v>
+      <c r="D115" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="116" spans="4:4">
-      <c r="D116" s="2" t="s">
-        <v>79</v>
+      <c r="D116" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="117" spans="4:4">
-      <c r="D117" s="2" t="s">
-        <v>80</v>
+      <c r="D117" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="118" spans="4:4">
-      <c r="D118" s="2" t="s">
-        <v>81</v>
+      <c r="D118" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="121" spans="4:4">
       <c r="D121" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="122" spans="4:4">
       <c r="D122" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="123" spans="4:4">
       <c r="D123" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="124" spans="4:4">
       <c r="D124" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="125" spans="4:4">
       <c r="D125" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="129" spans="4:4">
       <c r="D129" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="130" spans="4:4">
       <c r="D130" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="4:4">
       <c r="D131" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="132" spans="4:4">
       <c r="D132" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="133" spans="4:4">
       <c r="D133" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>